<commit_message>
... and further committee specifications from standards page
</commit_message>
<xml_diff>
--- a/oasis-standards.xlsx
+++ b/oasis-standards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdrees/merge_cisco_back_in/sdrees_at_oasis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686633E9-CC38-1145-B0A5-56ACF867B24D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209AE702-4D3B-9D42-8336-6648F2B6EE70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="0" windowWidth="25520" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4542" uniqueCount="2684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4612" uniqueCount="2696">
   <si>
     <t>AS4 Profile of ebMS 3.0 v1.0</t>
   </si>
@@ -8998,6 +8998,46 @@
   </si>
   <si>
     <t>Exchange Header Envelope (XHE) Version 1.0. Edited by G. Ken Holman. 21 March 2019. OASIS Committee Specification 01. https://docs.oasis-open.org/bdxr/xhe/v1.0/cs01/xhe-v1.0-cs01-oasis.html. Latest version: https://docs.oasis-open.org/bdxr/xhe/v1.0/xhe-v1.0-oasis.html.</t>
+  </si>
+  <si>
+    <t>https://www.oasis-open.org/committees/tc_home.php?wg_abbrev=ffm</t>
+  </si>
+  <si>
+    <t>Field Force Management Integration Interface Specification Version 1.0. 05 October 2012. OASIS Committee Specification 01.
+http://docs.oasis-open.org/ffm/FFMII-SPEC/v1.0/cs01/FFMII-SPEC-v1.0-cs01.html.</t>
+  </si>
+  <si>
+    <t>JSON Profile of XACML 3.0 Version 1.1</t>
+  </si>
+  <si>
+    <t>https://docs.oasis-open.org/xacml/xacml-json-http/v1.1/cs01/xacml-json-http-v1.1-cs01.html</t>
+  </si>
+  <si>
+    <t>https://docs.oasis-open.org/xacml/xacml-json-http/v1.1/cs01/xacml-json-http-v1.1-cs01.pdf</t>
+  </si>
+  <si>
+    <t>https://docs.oasis-open.org/xacml/xacml-json-http/v1.1/cs01/xacml-json-http-v1.1-cs01.doc</t>
+  </si>
+  <si>
+    <t>The aim of this profile is to define a standardized interface between a policy enforcement point and a policy decision point using JSON. The decision request and response structure is specified in the core XACML specification. This profile leverages it.</t>
+  </si>
+  <si>
+    <t>David Brossard (david.brossard@axiomatics.com), Axiomatics AB
+Steven Legg (steven.legg@viewds.com), Individual</t>
+  </si>
+  <si>
+    <t>https://docs.oasis-open.org/xacml/xacml-json-http/v1.1/cs01/xacml-json-http-v1.1-cs01.zip</t>
+  </si>
+  <si>
+    <t>https://www.oasis-open.org/committees/ballot.php?id=3278</t>
+  </si>
+  <si>
+    <t>[xacml-json-v1.1]</t>
+  </si>
+  <si>
+    <t>JSON Profile of XACML 3.0 Version 1.1. Edited by David Brossard and Steven Legg. 05 December 2018. OASIS Committee Specification 01.
+https://docs.oasis-open.org/xacml/xacml-json-http/v1.1/cs01/xacml-json-http-v1.1-cs01.html.
+Latest version: https://docs.oasis-open.org/xacml/xacml-json-http/v1.1/xacml-json-http-v1.1.html.</t>
   </si>
 </sst>
 </file>
@@ -9718,10 +9758,10 @@
   <dimension ref="A1:AF1498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F272" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F277" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C275" sqref="C275"/>
+      <selection pane="bottomRight" activeCell="C279" sqref="C279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28071,28 +28111,289 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="275" spans="1:31">
-      <c r="C275" s="2"/>
-      <c r="D275" s="20"/>
+    <row r="275" spans="1:31" s="7" customFormat="1" ht="409.6">
+      <c r="A275" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="B275" s="62" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C275" s="71" t="s">
+        <v>993</v>
+      </c>
+      <c r="D275" s="39" t="s">
+        <v>320</v>
+      </c>
       <c r="E275" s="82"/>
-      <c r="F275" s="6"/>
-      <c r="G275" s="10"/>
-    </row>
-    <row r="276" spans="1:31">
-      <c r="C276" s="4"/>
-      <c r="D276" s="22"/>
+      <c r="F275" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G275" s="10" t="s">
+        <v>994</v>
+      </c>
+      <c r="H275" s="10" t="s">
+        <v>995</v>
+      </c>
+      <c r="I275" s="10" t="s">
+        <v>996</v>
+      </c>
+      <c r="J275" s="8" t="s">
+        <v>998</v>
+      </c>
+      <c r="K275" s="70">
+        <v>41187</v>
+      </c>
+      <c r="L275" s="8" t="s">
+        <v>999</v>
+      </c>
+      <c r="M275" s="8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="N275" s="8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="O275" s="8"/>
+      <c r="P275" s="10" t="s">
+        <v>1002</v>
+      </c>
+      <c r="Q275" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="R275" s="8"/>
+      <c r="S275" s="8"/>
+      <c r="T275" s="10" t="s">
+        <v>1003</v>
+      </c>
+      <c r="U275" s="8"/>
+      <c r="V275" s="8"/>
+      <c r="W275" s="8"/>
+      <c r="X275" s="8"/>
+      <c r="Y275" s="7" t="s">
+        <v>1005</v>
+      </c>
+      <c r="Z275" s="11" t="s">
+        <v>2684</v>
+      </c>
+      <c r="AA275" s="79">
+        <v>41187</v>
+      </c>
+      <c r="AB275" s="11" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AD275" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AE275" s="8" t="s">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="276" spans="1:31" s="7" customFormat="1" ht="136">
+      <c r="A276" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="B276" s="62" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C276" s="71" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D276" s="40"/>
       <c r="E276" s="82"/>
-      <c r="F276" s="6"/>
-    </row>
-    <row r="277" spans="1:31">
+      <c r="F276" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G276" s="10" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H276" s="10" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I276" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J276" s="8" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K276" s="70">
+        <v>39534</v>
+      </c>
+      <c r="L276" s="8" t="s">
+        <v>1015</v>
+      </c>
+      <c r="M276" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="N276" s="8" t="s">
+        <v>1017</v>
+      </c>
+      <c r="O276" s="8"/>
+      <c r="P276" s="8"/>
+      <c r="Q276" s="8"/>
+      <c r="R276" s="8"/>
+      <c r="S276" s="8"/>
+      <c r="T276" s="8"/>
+      <c r="U276" s="8"/>
+      <c r="V276" s="8"/>
+      <c r="W276" s="8"/>
+      <c r="X276" s="8"/>
+      <c r="Y276" s="7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="Z276" s="11" t="s">
+        <v>1019</v>
+      </c>
+      <c r="AA276" s="79">
+        <v>39533</v>
+      </c>
+      <c r="AB276" s="11" t="s">
+        <v>1020</v>
+      </c>
+      <c r="AD276" s="7" t="s">
+        <v>1021</v>
+      </c>
+      <c r="AE276" s="8" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="277" spans="1:31" s="7" customFormat="1" ht="170">
+      <c r="A277" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="B277" s="62" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C277" s="71" t="s">
+        <v>2686</v>
+      </c>
+      <c r="D277" s="19" t="s">
+        <v>322</v>
+      </c>
       <c r="E277" s="82"/>
-      <c r="F277" s="6"/>
-    </row>
-    <row r="278" spans="1:31">
-      <c r="C278" s="2"/>
-      <c r="D278" s="20"/>
+      <c r="F277" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G277" s="10" t="s">
+        <v>2687</v>
+      </c>
+      <c r="H277" s="10" t="s">
+        <v>2688</v>
+      </c>
+      <c r="I277" s="10" t="s">
+        <v>2689</v>
+      </c>
+      <c r="J277" s="8"/>
+      <c r="K277" s="70">
+        <v>43439</v>
+      </c>
+      <c r="L277" s="8" t="s">
+        <v>2690</v>
+      </c>
+      <c r="M277" s="8" t="s">
+        <v>1029</v>
+      </c>
+      <c r="N277" s="8" t="s">
+        <v>2691</v>
+      </c>
+      <c r="O277" s="8"/>
+      <c r="P277" s="8"/>
+      <c r="Q277" s="8"/>
+      <c r="R277" s="8"/>
+      <c r="S277" s="8"/>
+      <c r="T277" s="10" t="s">
+        <v>2692</v>
+      </c>
+      <c r="U277" s="8"/>
+      <c r="V277" s="8"/>
+      <c r="W277" s="8"/>
+      <c r="X277" s="8"/>
+      <c r="Y277" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z277" s="11" t="s">
+        <v>1032</v>
+      </c>
+      <c r="AA277" s="79">
+        <v>43439</v>
+      </c>
+      <c r="AB277" s="11" t="s">
+        <v>2693</v>
+      </c>
+      <c r="AD277" s="7" t="s">
+        <v>2694</v>
+      </c>
+      <c r="AE277" s="8" t="s">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="278" spans="1:31" s="7" customFormat="1" ht="170">
+      <c r="A278" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="B278" s="62" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C278" s="28" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D278" s="39" t="s">
+        <v>320</v>
+      </c>
       <c r="E278" s="82"/>
-      <c r="F278" s="6"/>
+      <c r="F278" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G278" s="10" t="s">
+        <v>1024</v>
+      </c>
+      <c r="H278" s="10" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I278" s="10" t="s">
+        <v>1026</v>
+      </c>
+      <c r="J278" s="8"/>
+      <c r="K278" s="70">
+        <v>41984</v>
+      </c>
+      <c r="L278" s="8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="M278" s="8" t="s">
+        <v>1029</v>
+      </c>
+      <c r="N278" s="8" t="s">
+        <v>1030</v>
+      </c>
+      <c r="O278" s="8"/>
+      <c r="P278" s="8"/>
+      <c r="Q278" s="8"/>
+      <c r="R278" s="8"/>
+      <c r="S278" s="8"/>
+      <c r="T278" s="10" t="s">
+        <v>1031</v>
+      </c>
+      <c r="U278" s="8"/>
+      <c r="V278" s="8"/>
+      <c r="W278" s="8"/>
+      <c r="X278" s="8"/>
+      <c r="Y278" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z278" s="11" t="s">
+        <v>1032</v>
+      </c>
+      <c r="AA278" s="79">
+        <v>41984</v>
+      </c>
+      <c r="AB278" s="11" t="s">
+        <v>1033</v>
+      </c>
+      <c r="AD278" s="7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="AE278" s="8" t="s">
+        <v>1035</v>
+      </c>
     </row>
     <row r="279" spans="1:31">
       <c r="C279" s="4"/>
@@ -34742,24 +35043,87 @@
     </row>
   </sheetData>
   <mergeCells count="111">
-    <mergeCell ref="E1492:E1498"/>
-    <mergeCell ref="E1486:E1491"/>
-    <mergeCell ref="E1475:E1477"/>
-    <mergeCell ref="E1472:E1474"/>
-    <mergeCell ref="E1469:E1471"/>
-    <mergeCell ref="E1466:E1468"/>
-    <mergeCell ref="E1413:E1415"/>
-    <mergeCell ref="E1407:E1412"/>
-    <mergeCell ref="E1404:E1406"/>
-    <mergeCell ref="E1401:E1403"/>
-    <mergeCell ref="E1398:E1400"/>
-    <mergeCell ref="E1372:E1397"/>
-    <mergeCell ref="E1463:E1465"/>
-    <mergeCell ref="E1449:E1462"/>
-    <mergeCell ref="E1439:E1448"/>
-    <mergeCell ref="E1429:E1438"/>
-    <mergeCell ref="E1419:E1428"/>
-    <mergeCell ref="E1416:E1418"/>
+    <mergeCell ref="E112:E114"/>
+    <mergeCell ref="E289:E297"/>
+    <mergeCell ref="E273:E288"/>
+    <mergeCell ref="E347:E364"/>
+    <mergeCell ref="E342:E346"/>
+    <mergeCell ref="E337:E341"/>
+    <mergeCell ref="E322:E326"/>
+    <mergeCell ref="E301:E321"/>
+    <mergeCell ref="E298:E300"/>
+    <mergeCell ref="E424:E426"/>
+    <mergeCell ref="E400:E423"/>
+    <mergeCell ref="E395:E399"/>
+    <mergeCell ref="E389:E394"/>
+    <mergeCell ref="E384:E388"/>
+    <mergeCell ref="E365:E383"/>
+    <mergeCell ref="E472:E483"/>
+    <mergeCell ref="E463:E471"/>
+    <mergeCell ref="E446:E462"/>
+    <mergeCell ref="E434:E445"/>
+    <mergeCell ref="E431:E433"/>
+    <mergeCell ref="E427:E430"/>
+    <mergeCell ref="E573:E589"/>
+    <mergeCell ref="E533:E572"/>
+    <mergeCell ref="E501:E510"/>
+    <mergeCell ref="E495:E500"/>
+    <mergeCell ref="E488:E494"/>
+    <mergeCell ref="E484:E487"/>
+    <mergeCell ref="E630:E636"/>
+    <mergeCell ref="E617:E619"/>
+    <mergeCell ref="E610:E616"/>
+    <mergeCell ref="E603:E609"/>
+    <mergeCell ref="E593:E595"/>
+    <mergeCell ref="E590:E592"/>
+    <mergeCell ref="E668:E674"/>
+    <mergeCell ref="E661:E667"/>
+    <mergeCell ref="E654:E660"/>
+    <mergeCell ref="E647:E653"/>
+    <mergeCell ref="E644:E646"/>
+    <mergeCell ref="E637:E643"/>
+    <mergeCell ref="E710:E714"/>
+    <mergeCell ref="E703:E709"/>
+    <mergeCell ref="E696:E702"/>
+    <mergeCell ref="E689:E695"/>
+    <mergeCell ref="E682:E688"/>
+    <mergeCell ref="E675:E681"/>
+    <mergeCell ref="E908:E924"/>
+    <mergeCell ref="E898:E907"/>
+    <mergeCell ref="E870:E897"/>
+    <mergeCell ref="E849:E869"/>
+    <mergeCell ref="E739:E804"/>
+    <mergeCell ref="E715:E719"/>
+    <mergeCell ref="E968:E984"/>
+    <mergeCell ref="E961:E967"/>
+    <mergeCell ref="E958:E960"/>
+    <mergeCell ref="E943:E957"/>
+    <mergeCell ref="E928:E942"/>
+    <mergeCell ref="E925:E927"/>
+    <mergeCell ref="E1056:E1065"/>
+    <mergeCell ref="E1053:E1055"/>
+    <mergeCell ref="E1041:E1052"/>
+    <mergeCell ref="E1033:E1040"/>
+    <mergeCell ref="E1008:E1021"/>
+    <mergeCell ref="E985:E1007"/>
+    <mergeCell ref="E1117:E1119"/>
+    <mergeCell ref="E1112:E1116"/>
+    <mergeCell ref="E1107:E1111"/>
+    <mergeCell ref="E1095:E1099"/>
+    <mergeCell ref="E1074:E1078"/>
+    <mergeCell ref="E1066:E1073"/>
+    <mergeCell ref="E1174:E1182"/>
+    <mergeCell ref="E1169:E1173"/>
+    <mergeCell ref="E1166:E1168"/>
+    <mergeCell ref="E1149:E1160"/>
+    <mergeCell ref="E1125:E1148"/>
+    <mergeCell ref="E1120:E1124"/>
+    <mergeCell ref="E1237:E1239"/>
+    <mergeCell ref="E1234:E1236"/>
+    <mergeCell ref="E1231:E1233"/>
+    <mergeCell ref="E1228:E1230"/>
+    <mergeCell ref="E1186:E1227"/>
+    <mergeCell ref="E1183:E1185"/>
     <mergeCell ref="E1269:E1283"/>
     <mergeCell ref="E1266:E1268"/>
     <mergeCell ref="E1257:E1265"/>
@@ -34772,87 +35136,24 @@
     <mergeCell ref="E1298:E1328"/>
     <mergeCell ref="E1295:E1297"/>
     <mergeCell ref="E1284:E1294"/>
-    <mergeCell ref="E1174:E1182"/>
-    <mergeCell ref="E1169:E1173"/>
-    <mergeCell ref="E1166:E1168"/>
-    <mergeCell ref="E1149:E1160"/>
-    <mergeCell ref="E1125:E1148"/>
-    <mergeCell ref="E1120:E1124"/>
-    <mergeCell ref="E1237:E1239"/>
-    <mergeCell ref="E1234:E1236"/>
-    <mergeCell ref="E1231:E1233"/>
-    <mergeCell ref="E1228:E1230"/>
-    <mergeCell ref="E1186:E1227"/>
-    <mergeCell ref="E1183:E1185"/>
-    <mergeCell ref="E1056:E1065"/>
-    <mergeCell ref="E1053:E1055"/>
-    <mergeCell ref="E1041:E1052"/>
-    <mergeCell ref="E1033:E1040"/>
-    <mergeCell ref="E1008:E1021"/>
-    <mergeCell ref="E985:E1007"/>
-    <mergeCell ref="E1117:E1119"/>
-    <mergeCell ref="E1112:E1116"/>
-    <mergeCell ref="E1107:E1111"/>
-    <mergeCell ref="E1095:E1099"/>
-    <mergeCell ref="E1074:E1078"/>
-    <mergeCell ref="E1066:E1073"/>
-    <mergeCell ref="E908:E924"/>
-    <mergeCell ref="E898:E907"/>
-    <mergeCell ref="E870:E897"/>
-    <mergeCell ref="E849:E869"/>
-    <mergeCell ref="E739:E804"/>
-    <mergeCell ref="E715:E719"/>
-    <mergeCell ref="E968:E984"/>
-    <mergeCell ref="E961:E967"/>
-    <mergeCell ref="E958:E960"/>
-    <mergeCell ref="E943:E957"/>
-    <mergeCell ref="E928:E942"/>
-    <mergeCell ref="E925:E927"/>
-    <mergeCell ref="E668:E674"/>
-    <mergeCell ref="E661:E667"/>
-    <mergeCell ref="E654:E660"/>
-    <mergeCell ref="E647:E653"/>
-    <mergeCell ref="E644:E646"/>
-    <mergeCell ref="E637:E643"/>
-    <mergeCell ref="E710:E714"/>
-    <mergeCell ref="E703:E709"/>
-    <mergeCell ref="E696:E702"/>
-    <mergeCell ref="E689:E695"/>
-    <mergeCell ref="E682:E688"/>
-    <mergeCell ref="E675:E681"/>
-    <mergeCell ref="E573:E589"/>
-    <mergeCell ref="E533:E572"/>
-    <mergeCell ref="E501:E510"/>
-    <mergeCell ref="E495:E500"/>
-    <mergeCell ref="E488:E494"/>
-    <mergeCell ref="E484:E487"/>
-    <mergeCell ref="E630:E636"/>
-    <mergeCell ref="E617:E619"/>
-    <mergeCell ref="E610:E616"/>
-    <mergeCell ref="E603:E609"/>
-    <mergeCell ref="E593:E595"/>
-    <mergeCell ref="E590:E592"/>
-    <mergeCell ref="E424:E426"/>
-    <mergeCell ref="E400:E423"/>
-    <mergeCell ref="E395:E399"/>
-    <mergeCell ref="E389:E394"/>
-    <mergeCell ref="E384:E388"/>
-    <mergeCell ref="E365:E383"/>
-    <mergeCell ref="E472:E483"/>
-    <mergeCell ref="E463:E471"/>
-    <mergeCell ref="E446:E462"/>
-    <mergeCell ref="E434:E445"/>
-    <mergeCell ref="E431:E433"/>
-    <mergeCell ref="E427:E430"/>
-    <mergeCell ref="E112:E114"/>
-    <mergeCell ref="E289:E297"/>
-    <mergeCell ref="E273:E288"/>
-    <mergeCell ref="E347:E364"/>
-    <mergeCell ref="E342:E346"/>
-    <mergeCell ref="E337:E341"/>
-    <mergeCell ref="E322:E326"/>
-    <mergeCell ref="E301:E321"/>
-    <mergeCell ref="E298:E300"/>
+    <mergeCell ref="E1401:E1403"/>
+    <mergeCell ref="E1398:E1400"/>
+    <mergeCell ref="E1372:E1397"/>
+    <mergeCell ref="E1463:E1465"/>
+    <mergeCell ref="E1449:E1462"/>
+    <mergeCell ref="E1439:E1448"/>
+    <mergeCell ref="E1429:E1438"/>
+    <mergeCell ref="E1419:E1428"/>
+    <mergeCell ref="E1416:E1418"/>
+    <mergeCell ref="E1492:E1498"/>
+    <mergeCell ref="E1486:E1491"/>
+    <mergeCell ref="E1475:E1477"/>
+    <mergeCell ref="E1472:E1474"/>
+    <mergeCell ref="E1469:E1471"/>
+    <mergeCell ref="E1466:E1468"/>
+    <mergeCell ref="E1413:E1415"/>
+    <mergeCell ref="E1407:E1412"/>
+    <mergeCell ref="E1404:E1406"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -36409,10 +36710,35 @@
     <hyperlink ref="T274" r:id="rId1552" xr:uid="{9558B4FA-29AC-454A-BC53-15DBFA5E9C48}"/>
     <hyperlink ref="Z274" r:id="rId1553" xr:uid="{A80DFF42-7AF6-9343-9EAC-ADB5ABD09E94}"/>
     <hyperlink ref="AB274" r:id="rId1554" xr:uid="{192B9D4F-78EB-D64B-894A-EBA8B0032130}"/>
+    <hyperlink ref="G275" r:id="rId1555" xr:uid="{09861106-0A37-7F47-AEB3-161BF00ABAFA}"/>
+    <hyperlink ref="H275" r:id="rId1556" xr:uid="{B4FD611F-66E4-0942-938D-74BD71324ABD}"/>
+    <hyperlink ref="I275" r:id="rId1557" xr:uid="{BCF3CCDE-B3C6-E645-9E07-C90791D743C0}"/>
+    <hyperlink ref="Q275" r:id="rId1558" xr:uid="{7C5AE095-8311-E34C-8322-123119774307}"/>
+    <hyperlink ref="P275" r:id="rId1559" xr:uid="{1B6A10FC-E41B-6840-9EF3-67A0338F1ED6}"/>
+    <hyperlink ref="T275" r:id="rId1560" xr:uid="{B12068E2-016A-7141-8652-B7CD119892F5}"/>
+    <hyperlink ref="AB275" r:id="rId1561" xr:uid="{10514B07-9EE7-9E41-9E9B-4678574B46A5}"/>
+    <hyperlink ref="Z275" r:id="rId1562" xr:uid="{E0A0BE69-CE7A-714F-95C9-0359E5A431A9}"/>
+    <hyperlink ref="G276" r:id="rId1563" xr:uid="{777B17B8-7D2D-6849-8054-F4C25DCA38F4}"/>
+    <hyperlink ref="H276" r:id="rId1564" xr:uid="{48F2B37B-C17A-C148-A7D9-50887D78E731}"/>
+    <hyperlink ref="I276" r:id="rId1565" xr:uid="{07CC0966-A7B9-3E42-B11D-0FE98BE77F0F}"/>
+    <hyperlink ref="Z276" r:id="rId1566" xr:uid="{B22C4E1C-FCB3-244A-9E66-8D236C55E1B7}"/>
+    <hyperlink ref="AB276" r:id="rId1567" xr:uid="{81B1EDE6-D74E-B841-AF96-416F2B5850EE}"/>
+    <hyperlink ref="G277" r:id="rId1568" xr:uid="{B1BA2C76-5CFB-3440-A9CD-E77DC55D105B}"/>
+    <hyperlink ref="H277" r:id="rId1569" xr:uid="{8FCAF417-DB6C-8C4E-8271-81E27816E4FB}"/>
+    <hyperlink ref="I277" r:id="rId1570" xr:uid="{A25466AF-3964-FC44-86F0-5E7D998FA095}"/>
+    <hyperlink ref="T277" r:id="rId1571" xr:uid="{9AE16A33-7D74-D240-B429-5FFCAB83FA4E}"/>
+    <hyperlink ref="Z277" r:id="rId1572" xr:uid="{06CAE5AC-4E73-DC49-B45F-F03C26A7F1A3}"/>
+    <hyperlink ref="AB277" r:id="rId1573" xr:uid="{307942ED-7230-E040-9DD5-89032CE4C08C}"/>
+    <hyperlink ref="G278" r:id="rId1574" xr:uid="{9B829720-EBA7-AE44-B8E2-597AFBBAAF49}"/>
+    <hyperlink ref="H278" r:id="rId1575" xr:uid="{AF6D3C91-C20B-6240-B74A-084CA923CEC9}"/>
+    <hyperlink ref="I278" r:id="rId1576" xr:uid="{F129E287-87D7-ED48-A9F3-73C738526800}"/>
+    <hyperlink ref="T278" r:id="rId1577" xr:uid="{CCBB52C5-F484-A946-8805-21A1E35BAD07}"/>
+    <hyperlink ref="Z278" r:id="rId1578" xr:uid="{CCBE5F2A-A3FF-0A41-8246-B1F676952ABE}"/>
+    <hyperlink ref="AB278" r:id="rId1579" xr:uid="{B6B37849-21BD-6244-A16A-84545DBAE121}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1555"/>
+  <legacyDrawing r:id="rId1580"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>